<commit_message>
product coding completed. testing in pogress.
</commit_message>
<xml_diff>
--- a/soberano/test_cases/product_record_test_cases.xlsx
+++ b/soberano/test_cases/product_record_test_cases.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="83">
   <si>
     <t xml:space="preserve">TC Number</t>
   </si>
@@ -49,6 +49,9 @@
     <t xml:space="preserve">reference currency price</t>
   </si>
   <si>
+    <t xml:space="preserve">cost center</t>
+  </si>
+  <si>
     <t xml:space="preserve">test constrained (for input validation) form components</t>
   </si>
   <si>
@@ -64,6 +67,9 @@
     <t xml:space="preserve">mcat1</t>
   </si>
   <si>
+    <t xml:space="preserve">mcc4</t>
+  </si>
+  <si>
     <t xml:space="preserve">unit empty</t>
   </si>
   <si>
@@ -94,6 +100,9 @@
     <t xml:space="preserve">mcat2</t>
   </si>
   <si>
+    <t xml:space="preserve">mcc5</t>
+  </si>
+  <si>
     <t xml:space="preserve">User3 is NOT allowed to record product</t>
   </si>
   <si>
@@ -109,6 +118,9 @@
     <t xml:space="preserve">mcat3</t>
   </si>
   <si>
+    <t xml:space="preserve">mcc6</t>
+  </si>
+  <si>
     <t xml:space="preserve">User4 is allowed to record product</t>
   </si>
   <si>
@@ -127,6 +139,9 @@
     <t xml:space="preserve">mcat4</t>
   </si>
   <si>
+    <t xml:space="preserve">mcc7</t>
+  </si>
+  <si>
     <t xml:space="preserve">User6 is allowed to record product</t>
   </si>
   <si>
@@ -145,6 +160,9 @@
     <t xml:space="preserve">mcat5</t>
   </si>
   <si>
+    <t xml:space="preserve">mcc8</t>
+  </si>
+  <si>
     <t xml:space="preserve">User8 is allowed to record product</t>
   </si>
   <si>
@@ -157,6 +175,9 @@
     <t xml:space="preserve">mcat6</t>
   </si>
   <si>
+    <t xml:space="preserve">mcc9</t>
+  </si>
+  <si>
     <t xml:space="preserve">User9 is NOT allowed to record product</t>
   </si>
   <si>
@@ -172,6 +193,9 @@
     <t xml:space="preserve">mcat7</t>
   </si>
   <si>
+    <t xml:space="preserve">mcc10</t>
+  </si>
+  <si>
     <t xml:space="preserve">User10 is allowed to record product</t>
   </si>
   <si>
@@ -197,9 +221,6 @@
   </si>
   <si>
     <t xml:space="preserve">product9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mcat9</t>
   </si>
   <si>
     <t xml:space="preserve">User13 is NOT allowed to record product</t>
@@ -371,7 +392,7 @@
   <dimension ref="A1:AMJ32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7:J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -380,7 +401,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="55.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="5.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="6.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="6.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="8.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="10.88"/>
@@ -425,6 +446,9 @@
       <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="AMH1" s="1"/>
@@ -436,7 +460,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -444,22 +468,25 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" s="1" t="n">
         <v>1000</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H3" s="1" t="n">
         <v>1.001</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -467,22 +494,25 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>1000</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>1.001</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -490,22 +520,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>1000</v>
       </c>
       <c r="H5" s="1" t="n">
         <v>1.001</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -513,22 +546,25 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>1000</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -536,25 +572,28 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>1000</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H7" s="1" t="n">
         <v>1.001</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -562,25 +601,28 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>50.01234567</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H8" s="1" t="n">
         <v>2.00000002</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -588,25 +630,28 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F9" s="1" t="n">
         <v>1234.5678</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H9" s="1" t="n">
         <v>3.0123</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -614,25 +659,28 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="E10" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F10" s="1" t="n">
         <v>1234.5678</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H10" s="1" t="n">
         <v>3.0123</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -640,25 +688,28 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F11" s="1" t="n">
         <v>6543.21098</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="I11" s="1" t="n">
         <v>987.654</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -666,25 +717,28 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="D12" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F12" s="1" t="n">
         <v>6543.21098</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="I12" s="1" t="n">
         <v>987.654</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -692,25 +746,28 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F13" s="1" t="n">
         <v>7654321</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="I13" s="1" t="n">
         <v>876.123</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -718,25 +775,28 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F14" s="1" t="n">
         <v>12</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="I14" s="1" t="n">
         <v>3.45</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -744,25 +804,28 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="F15" s="1" t="n">
         <v>2</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="H15" s="1" t="n">
         <v>8.00998877</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -770,25 +833,28 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="F16" s="1" t="n">
         <v>2</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="H16" s="1" t="n">
         <v>8.00998877</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -796,25 +862,28 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="F17" s="1" t="n">
         <v>43526100</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="H17" s="1" t="n">
         <v>0.0005</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -822,25 +891,28 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F18" s="1" t="n">
         <v>12</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="H18" s="1" t="n">
         <v>1.09878901</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -848,25 +920,28 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F19" s="1" t="n">
         <v>12</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="H19" s="1" t="n">
         <v>1.09878901</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -874,25 +949,28 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F20" s="1" t="n">
         <v>12</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="H20" s="1" t="n">
         <v>1.09878901</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -900,25 +978,28 @@
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="F21" s="1" t="n">
         <v>234</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I21" s="1" t="n">
         <v>1234</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -926,25 +1007,28 @@
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="F22" s="1" t="n">
         <v>234</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I22" s="1" t="n">
         <v>1234</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -952,25 +1036,28 @@
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="F23" s="1" t="n">
         <v>234</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I23" s="1" t="n">
         <v>1234</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -978,7 +1065,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -986,7 +1073,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -994,7 +1081,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1002,7 +1089,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1010,7 +1097,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1018,7 +1105,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1026,7 +1113,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1034,7 +1121,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1042,7 +1129,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
now, when a ticket is printed:
on collecting: cash register printer has priority.
other cases: management printer.

product's unit change allowed, even if the new unit measure a different
magnitude. the stock's quantities are not converted if so (no conversion
factor to apply).
</commit_message>
<xml_diff>
--- a/soberano/test_cases/product_record_test_cases.xlsx
+++ b/soberano/test_cases/product_record_test_cases.xlsx
@@ -394,8 +394,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="8:8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>